<commit_message>
Modified the code and included more logic to compare the CSV files
</commit_message>
<xml_diff>
--- a/data/input/compare/mapping/Path_SDO_File Mapping V0.1.xlsx
+++ b/data/input/compare/mapping/Path_SDO_File Mapping V0.1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Workspace\CSV\csvutility\data\input\compare\mapping\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6858F8C-8745-4CD6-95D7-238CAA2E1489}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43603098-44A9-4C1B-80CB-C0246192DA4E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2304" yWindow="1884" windowWidth="20364" windowHeight="11076" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Mapping" sheetId="2" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="498" uniqueCount="233">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="504" uniqueCount="235">
   <si>
     <t>File Name</t>
   </si>
@@ -734,10 +734,16 @@
     <t>Prefix(Y)</t>
   </si>
   <si>
-    <t>STT_SDO_SLH_LAC_V1_EOD_NA_20201104212100.csv</t>
-  </si>
-  <si>
-    <t>accountpositions_market_20201104.csv</t>
+    <t>Tolerance(10)</t>
+  </si>
+  <si>
+    <t>Tolerance(20)</t>
+  </si>
+  <si>
+    <t>Prod_PATH.csv</t>
+  </si>
+  <si>
+    <t>QA_PATH.csv</t>
   </si>
 </sst>
 </file>
@@ -1908,8 +1914,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4DB49C5B-9919-45C5-9892-FFA12CF07D74}">
   <dimension ref="A1:G58"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1951,13 +1957,13 @@
         <v>218</v>
       </c>
       <c r="B2" t="s">
-        <v>231</v>
-      </c>
-      <c r="C2" s="11" t="s">
-        <v>6</v>
+        <v>233</v>
+      </c>
+      <c r="C2" t="s">
+        <v>7</v>
       </c>
       <c r="D2" t="s">
-        <v>232</v>
+        <v>234</v>
       </c>
       <c r="E2" t="s">
         <v>7</v>
@@ -1970,22 +1976,25 @@
       <c r="A3" t="s">
         <v>218</v>
       </c>
-      <c r="C3" s="12" t="s">
-        <v>21</v>
+      <c r="C3" s="1" t="s">
+        <v>8</v>
       </c>
       <c r="E3" s="1" t="s">
         <v>8</v>
+      </c>
+      <c r="F3" s="15" t="s">
+        <v>228</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>218</v>
       </c>
-      <c r="C4" s="11" t="s">
-        <v>11</v>
+      <c r="C4" s="1" t="s">
+        <v>140</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>11</v>
+        <v>140</v>
       </c>
       <c r="G4" t="s">
         <v>230</v>
@@ -1995,19 +2004,22 @@
       <c r="A5" t="s">
         <v>218</v>
       </c>
-      <c r="C5" s="11" t="s">
-        <v>31</v>
+      <c r="C5" s="1" t="s">
+        <v>124</v>
       </c>
       <c r="E5" s="1" t="s">
         <v>124</v>
+      </c>
+      <c r="G5" t="s">
+        <v>231</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>218</v>
       </c>
-      <c r="C6" s="13" t="s">
-        <v>29</v>
+      <c r="C6" s="1" t="s">
+        <v>147</v>
       </c>
       <c r="E6" s="1" t="s">
         <v>147</v>
@@ -2018,8 +2030,8 @@
       <c r="A7" t="s">
         <v>218</v>
       </c>
-      <c r="C7" s="11" t="s">
-        <v>30</v>
+      <c r="C7" s="1" t="s">
+        <v>148</v>
       </c>
       <c r="E7" s="1" t="s">
         <v>148</v>
@@ -2030,10 +2042,13 @@
         <v>218</v>
       </c>
       <c r="C8" s="6" t="s">
-        <v>35</v>
+        <v>145</v>
       </c>
       <c r="E8" s="6" t="s">
-        <v>128</v>
+        <v>145</v>
+      </c>
+      <c r="G8" t="s">
+        <v>232</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.3">
@@ -2041,18 +2056,21 @@
         <v>218</v>
       </c>
       <c r="C9" s="6" t="s">
-        <v>38</v>
+        <v>129</v>
       </c>
       <c r="E9" s="6" t="s">
         <v>129</v>
+      </c>
+      <c r="G9" t="s">
+        <v>232</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>218</v>
       </c>
-      <c r="C10" s="6" t="s">
-        <v>36</v>
+      <c r="C10" s="1" t="s">
+        <v>194</v>
       </c>
       <c r="E10" s="1" t="s">
         <v>194</v>
@@ -2062,8 +2080,8 @@
       <c r="A11" t="s">
         <v>218</v>
       </c>
-      <c r="C11" s="6" t="s">
-        <v>37</v>
+      <c r="C11" s="1" t="s">
+        <v>195</v>
       </c>
       <c r="E11" s="1" t="s">
         <v>195</v>
@@ -2074,10 +2092,13 @@
         <v>218</v>
       </c>
       <c r="C12" s="6" t="s">
-        <v>42</v>
+        <v>130</v>
       </c>
       <c r="E12" s="6" t="s">
         <v>130</v>
+      </c>
+      <c r="G12" t="s">
+        <v>232</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.3">
@@ -2085,7 +2106,7 @@
         <v>218</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>40</v>
+        <v>196</v>
       </c>
       <c r="E13" s="1" t="s">
         <v>196</v>
@@ -2096,18 +2117,21 @@
         <v>218</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>41</v>
+        <v>197</v>
       </c>
       <c r="E14" s="1" t="s">
         <v>197</v>
+      </c>
+      <c r="G14" t="s">
+        <v>232</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>218</v>
       </c>
-      <c r="C15" s="6" t="s">
-        <v>46</v>
+      <c r="C15" s="1" t="s">
+        <v>131</v>
       </c>
       <c r="E15" s="1" t="s">
         <v>131</v>
@@ -2117,8 +2141,8 @@
       <c r="A16" t="s">
         <v>218</v>
       </c>
-      <c r="C16" s="6" t="s">
-        <v>49</v>
+      <c r="C16" s="1" t="s">
+        <v>132</v>
       </c>
       <c r="E16" s="1" t="s">
         <v>132</v>
@@ -2129,7 +2153,7 @@
         <v>218</v>
       </c>
       <c r="C17" s="6" t="s">
-        <v>53</v>
+        <v>134</v>
       </c>
       <c r="E17" s="6" t="s">
         <v>134</v>
@@ -2140,7 +2164,7 @@
         <v>218</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>51</v>
+        <v>202</v>
       </c>
       <c r="E18" s="1" t="s">
         <v>202</v>
@@ -2151,7 +2175,7 @@
         <v>218</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>52</v>
+        <v>201</v>
       </c>
       <c r="E19" s="1" t="s">
         <v>201</v>
@@ -2162,7 +2186,7 @@
         <v>218</v>
       </c>
       <c r="C20" s="6" t="s">
-        <v>56</v>
+        <v>133</v>
       </c>
       <c r="E20" s="6" t="s">
         <v>133</v>
@@ -2173,7 +2197,7 @@
         <v>218</v>
       </c>
       <c r="C21" t="s">
-        <v>54</v>
+        <v>173</v>
       </c>
       <c r="E21" t="s">
         <v>173</v>
@@ -2183,8 +2207,8 @@
       <c r="A22" t="s">
         <v>218</v>
       </c>
-      <c r="C22" s="6" t="s">
-        <v>68</v>
+      <c r="C22" s="1" t="s">
+        <v>127</v>
       </c>
       <c r="E22" s="1" t="s">
         <v>127</v>
@@ -2195,10 +2219,10 @@
         <v>218</v>
       </c>
       <c r="C23" s="6" t="s">
-        <v>84</v>
+        <v>141</v>
       </c>
       <c r="E23" s="6" t="s">
-        <v>135</v>
+        <v>141</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.3">
@@ -2387,6 +2411,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>